<commit_message>
Need to edit output path
</commit_message>
<xml_diff>
--- a/Southface_python/Data/test_input.xlsx
+++ b/Southface_python/Data/test_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdelk\OneDrive - Southface\Documents\VS_Code\Southface_python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zdelk\OneDrive - Southface\Documents\VS_Code\Southface_python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BC1C47-16F4-4733-B488-2F2627356833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77928AE-8FEF-4B7D-965D-DC6C80A145B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10560" activeTab="1" xr2:uid="{9F5AF8BB-9AFE-4307-BB09-5A031DC3E34F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{9F5AF8BB-9AFE-4307-BB09-5A031DC3E34F}"/>
   </bookViews>
   <sheets>
     <sheet name="Utility Bills" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,25 @@
     <sheet name="Pipe Data" sheetId="2" r:id="rId3"/>
     <sheet name="VSD Replacement" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="146">
   <si>
     <t>month</t>
   </si>
@@ -196,9 +209,6 @@
     <t>air_staff_needed</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>uptime_factory</t>
   </si>
   <si>
@@ -406,39 +416,24 @@
     <t>type</t>
   </si>
   <si>
-    <t>Gas</t>
-  </si>
-  <si>
     <t>Gas Charge ($)</t>
   </si>
   <si>
     <t>Gas Usage</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t>Air Leak Variables Full</t>
   </si>
   <si>
-    <t>Air Leak Var</t>
-  </si>
-  <si>
     <t>FC Var</t>
   </si>
   <si>
     <t>Facility Variables Full</t>
   </si>
   <si>
-    <t>AL Values</t>
-  </si>
-  <si>
     <t>Pipe Var</t>
   </si>
   <si>
-    <t>Pipe Values</t>
-  </si>
-  <si>
     <t>LED Var</t>
   </si>
   <si>
@@ -467,6 +462,18 @@
   </si>
   <si>
     <t>FC Value</t>
+  </si>
+  <si>
+    <t>Pipe Value</t>
+  </si>
+  <si>
+    <t>AirLeak Var</t>
+  </si>
+  <si>
+    <t>AirLeak Value</t>
+  </si>
+  <si>
+    <t>Electric</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1339,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1362,13 +1369,13 @@
         <v>46</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -1396,11 +1403,11 @@
       <c r="F2">
         <v>6769.12</v>
       </c>
-      <c r="G2" t="s">
-        <v>130</v>
-      </c>
-      <c r="H2" t="s">
-        <v>130</v>
+      <c r="G2">
+        <v>5000</v>
+      </c>
+      <c r="H2">
+        <v>8950</v>
       </c>
       <c r="I2">
         <v>288.49</v>
@@ -1428,11 +1435,11 @@
       <c r="F3">
         <v>7447.17</v>
       </c>
-      <c r="G3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" t="s">
-        <v>130</v>
+      <c r="G3">
+        <v>4600</v>
+      </c>
+      <c r="H3">
+        <v>8234</v>
       </c>
       <c r="I3">
         <v>301.51</v>
@@ -1460,11 +1467,11 @@
       <c r="F4">
         <v>9367.7999999999993</v>
       </c>
-      <c r="G4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" t="s">
-        <v>130</v>
+      <c r="G4">
+        <v>7320</v>
+      </c>
+      <c r="H4">
+        <v>13102.800000000001</v>
       </c>
       <c r="I4">
         <v>333.26</v>
@@ -1492,11 +1499,11 @@
       <c r="F5">
         <v>8379.99</v>
       </c>
-      <c r="G5" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" t="s">
-        <v>130</v>
+      <c r="G5">
+        <v>7960</v>
+      </c>
+      <c r="H5">
+        <v>14248.4</v>
       </c>
       <c r="I5">
         <v>381.51</v>
@@ -1524,11 +1531,11 @@
       <c r="F6">
         <v>7656.69</v>
       </c>
-      <c r="G6" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" t="s">
-        <v>130</v>
+      <c r="G6">
+        <v>9120</v>
+      </c>
+      <c r="H6">
+        <v>16324.800000000001</v>
       </c>
       <c r="I6">
         <v>341.92</v>
@@ -1556,11 +1563,11 @@
       <c r="F7">
         <v>9047.9599999999991</v>
       </c>
-      <c r="G7" t="s">
-        <v>130</v>
-      </c>
-      <c r="H7" t="s">
-        <v>130</v>
+      <c r="G7">
+        <v>10280</v>
+      </c>
+      <c r="H7">
+        <v>18401.2</v>
       </c>
       <c r="I7">
         <v>378.62</v>
@@ -1588,11 +1595,11 @@
       <c r="F8">
         <v>8249.2199999999993</v>
       </c>
-      <c r="G8" t="s">
-        <v>130</v>
-      </c>
-      <c r="H8" t="s">
-        <v>130</v>
+      <c r="G8">
+        <v>11440</v>
+      </c>
+      <c r="H8">
+        <v>20477.600000000002</v>
       </c>
       <c r="I8">
         <v>414.91</v>
@@ -1620,11 +1627,11 @@
       <c r="F9">
         <v>8835.3700000000008</v>
       </c>
-      <c r="G9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H9" t="s">
-        <v>130</v>
+      <c r="G9">
+        <v>12600</v>
+      </c>
+      <c r="H9">
+        <v>22554</v>
       </c>
       <c r="I9">
         <v>349.1</v>
@@ -1652,11 +1659,11 @@
       <c r="F10">
         <v>8585.01</v>
       </c>
-      <c r="G10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H10" t="s">
-        <v>130</v>
+      <c r="G10">
+        <v>13760</v>
+      </c>
+      <c r="H10">
+        <v>24630.400000000001</v>
       </c>
       <c r="I10">
         <v>547.25</v>
@@ -1684,11 +1691,11 @@
       <c r="F11">
         <v>8815.36</v>
       </c>
-      <c r="G11" t="s">
-        <v>130</v>
-      </c>
-      <c r="H11" t="s">
-        <v>130</v>
+      <c r="G11">
+        <v>14920</v>
+      </c>
+      <c r="H11">
+        <v>26706.799999999999</v>
       </c>
       <c r="I11">
         <v>271.73</v>
@@ -1716,11 +1723,11 @@
       <c r="F12">
         <v>8335.81</v>
       </c>
-      <c r="G12" t="s">
-        <v>130</v>
-      </c>
-      <c r="H12" t="s">
-        <v>130</v>
+      <c r="G12">
+        <v>16080</v>
+      </c>
+      <c r="H12">
+        <v>28783.200000000001</v>
       </c>
       <c r="I12">
         <v>299.06</v>
@@ -1748,11 +1755,11 @@
       <c r="F13">
         <v>8096.8</v>
       </c>
-      <c r="G13" t="s">
-        <v>130</v>
-      </c>
-      <c r="H13" t="s">
-        <v>130</v>
+      <c r="G13">
+        <v>17240</v>
+      </c>
+      <c r="H13">
+        <v>30859.600000000002</v>
       </c>
       <c r="I13">
         <v>290.93</v>
@@ -1770,8 +1777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E70CBA-8199-4A3A-AFAC-CD5C15AA56F2}">
   <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,52 +1797,49 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="M1" t="s">
+        <v>137</v>
+      </c>
+      <c r="N1" t="s">
+        <v>132</v>
+      </c>
+      <c r="O1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E1" t="s">
-        <v>131</v>
-      </c>
-      <c r="F1" t="s">
-        <v>132</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="S1" t="s">
         <v>135</v>
-      </c>
-      <c r="I1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" t="s">
-        <v>136</v>
-      </c>
-      <c r="K1" t="s">
-        <v>137</v>
-      </c>
-      <c r="M1" t="s">
-        <v>143</v>
-      </c>
-      <c r="N1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O1" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>142</v>
-      </c>
-      <c r="R1" t="s">
-        <v>140</v>
-      </c>
-      <c r="S1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -1843,13 +1847,13 @@
         <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1">
         <v>6240</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>50</v>
@@ -1858,28 +1862,28 @@
         <v>0.9</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="K2" s="1">
         <v>0.8</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O2" s="1">
         <v>75</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="S2" s="1">
         <v>0.74560000000000004</v>
@@ -1890,13 +1894,13 @@
         <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>51</v>
@@ -1905,28 +1909,28 @@
         <v>0.61</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="K3" s="1" t="s">
-        <v>127</v>
+        <v>145</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O3" s="1">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="Q3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="S3" s="2">
         <v>45000</v>
@@ -1934,7 +1938,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>52</v>
@@ -1943,28 +1947,28 @@
         <v>90</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="K4" s="2">
         <v>0.3</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="O4" s="1">
         <v>1700</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S4" s="2">
         <v>22500</v>
@@ -1972,28 +1976,28 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="G5" s="1">
         <v>933</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="K5" s="2">
         <v>0.32</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="O5" s="2">
         <v>50000</v>
@@ -2001,7 +2005,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>53</v>
@@ -2010,19 +2014,19 @@
         <v>1.3500000000000001E-3</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K6" s="2">
         <v>2</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O6" s="2">
         <v>24000</v>
@@ -2030,7 +2034,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>54</v>
@@ -2039,19 +2043,19 @@
         <v>20</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K7" s="2">
         <v>1.5</v>
       </c>
       <c r="M7" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="O7" s="2">
         <v>40000</v>
@@ -2059,7 +2063,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>55</v>
@@ -2068,19 +2072,19 @@
         <v>8</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="K8" s="2">
         <v>0.12</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O8" s="2">
         <v>9.24</v>
@@ -2088,7 +2092,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>56</v>
@@ -2097,19 +2101,19 @@
         <v>2</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="K9" s="2">
         <v>91.63</v>
       </c>
       <c r="M9" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="O9" s="2">
         <v>11.96</v>
@@ -2117,28 +2121,28 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="G10" s="2">
         <v>1.4</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="K10" s="2">
         <v>9.5299999999999994</v>
       </c>
       <c r="M10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="O10" s="2">
         <v>6.67</v>
@@ -2146,28 +2150,28 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="G11" s="2">
         <v>1.4</v>
       </c>
       <c r="I11" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="K11" s="2">
         <v>133</v>
       </c>
       <c r="M11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="O11" s="2">
         <v>142</v>
@@ -2175,19 +2179,19 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G12" s="2">
         <v>101</v>
       </c>
       <c r="M12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="O12" s="2">
         <v>13.9</v>
@@ -2195,10 +2199,10 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="2">
         <v>0.28699999999999998</v>
@@ -2206,10 +2210,10 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="G14" s="2">
         <v>5000</v>
@@ -2217,10 +2221,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G15" s="2">
         <v>30</v>

</xml_diff>